<commit_message>
new features were inserted into version2
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -11,15 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>YOUR GMAIL</t>
+  </si>
   <si>
     <t>ACCOUNT NAME</t>
   </si>
   <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
+    <t>PINTEREST EMAIL</t>
+  </si>
+  <si>
+    <t>PINTEREST PASSWORD</t>
   </si>
   <si>
     <t>PINS TITLE</t>
@@ -28,12 +31,15 @@
     <t>PINS DESCRIPTION</t>
   </si>
   <si>
-    <t>LINK</t>
+    <t>PINS LINK</t>
   </si>
   <si>
     <t>PATH TO IMAGES</t>
   </si>
   <si>
+    <t>user-example-mail@gmail.com</t>
+  </si>
+  <si>
     <t>Cakes_Account</t>
   </si>
   <si>
@@ -49,7 +55,7 @@
     <t>Make a bigger cake than anyone</t>
   </si>
   <si>
-    <t>https://www.amazon.com/</t>
+    <t>https://www.hugecakesexample.com/</t>
   </si>
   <si>
     <t>"C:\Documents\fotos_tortas"</t>
@@ -334,11 +340,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.38"/>
-    <col customWidth="1" min="2" max="2" width="24.5"/>
-    <col customWidth="1" min="3" max="5" width="21.0"/>
-    <col customWidth="1" min="6" max="6" width="25.63"/>
-    <col customWidth="1" min="7" max="7" width="28.75"/>
+    <col customWidth="1" min="1" max="2" width="15.38"/>
+    <col customWidth="1" min="3" max="3" width="24.5"/>
+    <col customWidth="1" min="4" max="6" width="21.0"/>
+    <col customWidth="1" min="7" max="7" width="25.63"/>
+    <col customWidth="1" min="8" max="8" width="28.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -363,28 +369,34 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -394,6 +406,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="4"/>
@@ -403,6 +416,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="4"/>
@@ -412,6 +426,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="4"/>
@@ -421,6 +436,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="4"/>
@@ -430,6 +446,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="4"/>
@@ -439,6 +456,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="4"/>
@@ -448,6 +466,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="4"/>
@@ -457,6 +476,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="4"/>
@@ -466,10 +486,11 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink r:id="rId1" ref="G2"/>
   </hyperlinks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>